<commit_message>
Added index files and working on adding terms to index
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w76c139\Box Sync\Greenwood_Book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>Index terms</t>
   </si>
@@ -204,14 +204,58 @@
   </si>
   <si>
     <t>cell means</t>
+  </si>
+  <si>
+    <t>Added to:</t>
+  </si>
+  <si>
+    <t>Chapter 1</t>
+  </si>
+  <si>
+    <t>Chapter 2</t>
+  </si>
+  <si>
+    <t>Chapter 3</t>
+  </si>
+  <si>
+    <t>Chapter 4</t>
+  </si>
+  <si>
+    <t>Chapter 5</t>
+  </si>
+  <si>
+    <t>Chapter 6</t>
+  </si>
+  <si>
+    <t>Chapter 7</t>
+  </si>
+  <si>
+    <t>Chapter 8</t>
+  </si>
+  <si>
+    <t>Chapter 9</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -239,8 +283,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,302 +566,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="32.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding index terms to chapter 2
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8D9DFB48-F6C0-4C3C-A369-2F4569F3694D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="74">
   <si>
     <t>Index terms</t>
   </si>
@@ -251,7 +252,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,11 +572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -803,6 +804,9 @@
       <c r="B19" t="s">
         <v>70</v>
       </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
@@ -811,6 +815,9 @@
       <c r="B20" t="s">
         <v>70</v>
       </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -819,6 +826,9 @@
       <c r="B21" t="s">
         <v>70</v>
       </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
@@ -826,6 +836,9 @@
       </c>
       <c r="B22" t="s">
         <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Polished some index terms, finished chapter 2 layout, adding index terms to chapter 3
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{425AD61B-D8E2-47AF-8E8E-AD2E7A87D41D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7DFCA71C-83F3-431A-82ED-0A10C41AB7CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="76">
   <si>
     <t>Index terms</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>import data</t>
+  </si>
+  <si>
+    <t>permutation!distribution</t>
+  </si>
+  <si>
+    <t>permutation!test</t>
   </si>
 </sst>
 </file>
@@ -573,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -631,6 +637,9 @@
       <c r="C3" t="s">
         <v>72</v>
       </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -642,6 +651,9 @@
       <c r="C4" t="s">
         <v>70</v>
       </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -653,6 +665,9 @@
       <c r="C5" t="s">
         <v>72</v>
       </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -664,6 +679,9 @@
       <c r="C6" t="s">
         <v>72</v>
       </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -675,6 +693,9 @@
       <c r="C7" t="s">
         <v>72</v>
       </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -686,6 +707,9 @@
       <c r="C8" t="s">
         <v>72</v>
       </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -697,6 +721,9 @@
       <c r="C9" t="s">
         <v>72</v>
       </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -708,6 +735,9 @@
       <c r="C10" t="s">
         <v>72</v>
       </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -719,6 +749,9 @@
       <c r="C11" t="s">
         <v>70</v>
       </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -730,6 +763,9 @@
       <c r="C12" t="s">
         <v>70</v>
       </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -741,6 +777,9 @@
       <c r="C13" t="s">
         <v>70</v>
       </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -752,6 +791,9 @@
       <c r="C14" t="s">
         <v>70</v>
       </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -763,6 +805,9 @@
       <c r="C15" t="s">
         <v>70</v>
       </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -774,8 +819,11 @@
       <c r="C16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -785,8 +833,11 @@
       <c r="C17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -796,8 +847,11 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -807,440 +861,557 @@
       <c r="C19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>43</v>
       </c>
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>71</v>
       </c>
-      <c r="C41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>51</v>
       </c>
-      <c r="B46" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+      <c r="B49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>57</v>
       </c>
-      <c r="B48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>58</v>
       </c>
-      <c r="B49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>59</v>
       </c>
-      <c r="B50" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>73</v>
       </c>
-      <c r="B51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>11</v>
       </c>
-      <c r="B54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>12</v>
       </c>
-      <c r="B55" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>13</v>
       </c>
-      <c r="B56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="B58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>14</v>
       </c>
-      <c r="B57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>21</v>
       </c>
-      <c r="B58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>27</v>
       </c>
-      <c r="B59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>28</v>
       </c>
-      <c r="B60" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>29</v>
       </c>
-      <c r="B61" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>52</v>
       </c>
-      <c r="B62" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>54</v>
-      </c>
       <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
@@ -1251,9 +1422,34 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
+        <v>54</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>55</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished adding index terms to chapter 3, fixed page layouts
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7DFCA71C-83F3-431A-82ED-0A10C41AB7CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1517BA0F-6EB3-4603-BDE8-EF426A4FF08C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="85">
   <si>
     <t>Index terms</t>
   </si>
@@ -253,6 +253,33 @@
   </si>
   <si>
     <t>permutation!test</t>
+  </si>
+  <si>
+    <t>p-value!calculation of</t>
+  </si>
+  <si>
+    <t>p-value!criticisim</t>
+  </si>
+  <si>
+    <t>p-value!one-sided test</t>
+  </si>
+  <si>
+    <t>p-value!permutation distribution</t>
+  </si>
+  <si>
+    <t>p-value!strength of evidence</t>
+  </si>
+  <si>
+    <t>p-value!two-sided test</t>
+  </si>
+  <si>
+    <t>p-value!zero</t>
+  </si>
+  <si>
+    <t>p-value!interpretation of</t>
+  </si>
+  <si>
+    <t>pdata</t>
   </si>
 </sst>
 </file>
@@ -579,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1183,273 +1210,474 @@
       <c r="C42" t="s">
         <v>72</v>
       </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
         <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
         <v>70</v>
       </c>
       <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>51</v>
       </c>
-      <c r="B48" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B50" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="B58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B51" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B52" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>73</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B61" t="s">
         <v>71</v>
       </c>
-      <c r="C53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
+      <c r="C61" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>11</v>
       </c>
-      <c r="B56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
         <v>12</v>
       </c>
-      <c r="B57" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
         <v>13</v>
       </c>
-      <c r="B58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>14</v>
       </c>
-      <c r="B59" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>21</v>
       </c>
-      <c r="B60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>27</v>
       </c>
-      <c r="B61" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>28</v>
       </c>
-      <c r="B62" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>29</v>
       </c>
-      <c r="B63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>52</v>
       </c>
-      <c r="B64" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>53</v>
       </c>
-      <c r="B65" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
         <v>54</v>
       </c>
-      <c r="B66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="B75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
         <v>19</v>
       </c>
-      <c r="B67" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+      <c r="B76" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>55</v>
       </c>
-      <c r="B68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C77" t="s">
+        <v>70</v>
+      </c>
+      <c r="D77" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding index terms to chapter 4. Renumbered plots in chapter
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1517BA0F-6EB3-4603-BDE8-EF426A4FF08C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E1F6E3E0-02F6-4643-84CB-2AD7D291BF67}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="85">
   <si>
     <t>Index terms</t>
   </si>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -667,6 +667,9 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -681,6 +684,9 @@
       <c r="D4" t="s">
         <v>70</v>
       </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -695,6 +701,9 @@
       <c r="D5" t="s">
         <v>70</v>
       </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -709,6 +718,9 @@
       <c r="D6" t="s">
         <v>72</v>
       </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -723,6 +735,9 @@
       <c r="D7" t="s">
         <v>70</v>
       </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -737,6 +752,9 @@
       <c r="D8" t="s">
         <v>70</v>
       </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -751,6 +769,9 @@
       <c r="D9" t="s">
         <v>72</v>
       </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -765,6 +786,9 @@
       <c r="D10" t="s">
         <v>70</v>
       </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -779,6 +803,9 @@
       <c r="D11" t="s">
         <v>70</v>
       </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -793,6 +820,9 @@
       <c r="D12" t="s">
         <v>72</v>
       </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -807,6 +837,9 @@
       <c r="D13" t="s">
         <v>70</v>
       </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -821,6 +854,9 @@
       <c r="D14" t="s">
         <v>70</v>
       </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -835,6 +871,9 @@
       <c r="D15" t="s">
         <v>70</v>
       </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -849,8 +888,11 @@
       <c r="D16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -863,8 +905,11 @@
       <c r="D17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -877,8 +922,11 @@
       <c r="D18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -891,8 +939,11 @@
       <c r="D19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -905,8 +956,11 @@
       <c r="D20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -919,8 +973,11 @@
       <c r="D21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -933,8 +990,11 @@
       <c r="D22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -947,8 +1007,11 @@
       <c r="D23" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -961,8 +1024,11 @@
       <c r="D24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -975,8 +1041,11 @@
       <c r="D25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -989,8 +1058,11 @@
       <c r="D26" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1003,8 +1075,11 @@
       <c r="D27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1017,8 +1092,11 @@
       <c r="D28" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1031,8 +1109,11 @@
       <c r="D29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1045,8 +1126,11 @@
       <c r="D30" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1059,8 +1143,11 @@
       <c r="D31" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1073,8 +1160,11 @@
       <c r="D32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1087,8 +1177,11 @@
       <c r="D33" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1101,8 +1194,11 @@
       <c r="D34" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1115,8 +1211,11 @@
       <c r="D35" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1129,8 +1228,11 @@
       <c r="D36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1143,8 +1245,11 @@
       <c r="D37" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1157,8 +1262,11 @@
       <c r="D38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1171,8 +1279,11 @@
       <c r="D39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1185,8 +1296,11 @@
       <c r="D40" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1199,8 +1313,11 @@
       <c r="D41" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1213,8 +1330,11 @@
       <c r="D42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -1227,8 +1347,11 @@
       <c r="D43" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -1241,8 +1364,11 @@
       <c r="D44" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -1255,8 +1381,11 @@
       <c r="D45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -1269,8 +1398,11 @@
       <c r="D46" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -1283,8 +1415,11 @@
       <c r="D47" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -1297,8 +1432,11 @@
       <c r="D48" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -1311,8 +1449,11 @@
       <c r="D49" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -1325,8 +1466,11 @@
       <c r="D50" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -1339,8 +1483,11 @@
       <c r="D51" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -1353,8 +1500,11 @@
       <c r="D52" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -1367,8 +1517,11 @@
       <c r="D53" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1381,8 +1534,11 @@
       <c r="D54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -1395,8 +1551,11 @@
       <c r="D55" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1409,8 +1568,11 @@
       <c r="D56" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1423,8 +1585,11 @@
       <c r="D57" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1437,8 +1602,11 @@
       <c r="D58" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1451,8 +1619,11 @@
       <c r="D59" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1465,8 +1636,11 @@
       <c r="D60" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -1479,13 +1653,16 @@
       <c r="D61" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Finished adding index terms to chapter 4. Adjusted page layout
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E1F6E3E0-02F6-4643-84CB-2AD7D291BF67}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AB47831-CC34-4FCF-8162-0E5D205B684F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="85">
   <si>
     <t>Index terms</t>
   </si>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1144,7 +1144,7 @@
         <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -1675,8 +1675,11 @@
       <c r="D64" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -1689,8 +1692,11 @@
       <c r="D65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -1703,8 +1709,11 @@
       <c r="D66" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -1717,8 +1726,11 @@
       <c r="D67" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>21</v>
       </c>
@@ -1731,8 +1743,11 @@
       <c r="D68" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>27</v>
       </c>
@@ -1745,8 +1760,11 @@
       <c r="D69" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -1759,8 +1777,11 @@
       <c r="D70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>29</v>
       </c>
@@ -1773,8 +1794,11 @@
       <c r="D71" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -1787,8 +1811,11 @@
       <c r="D72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>53</v>
       </c>
@@ -1801,8 +1828,11 @@
       <c r="D73" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -1815,8 +1845,11 @@
       <c r="D74" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>54</v>
       </c>
@@ -1829,8 +1862,11 @@
       <c r="D75" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -1843,8 +1879,11 @@
       <c r="D76" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -1856,6 +1895,9 @@
       </c>
       <c r="D77" t="s">
         <v>70</v>
+      </c>
+      <c r="E77" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made tableplot one word, finished adding index terms for chapter 5
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AB47831-CC34-4FCF-8162-0E5D205B684F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68AE027A-8891-46E5-97E0-31B6824F485E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="85">
   <si>
     <t>Index terms</t>
   </si>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -670,6 +670,9 @@
       <c r="E3" t="s">
         <v>72</v>
       </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -687,6 +690,9 @@
       <c r="E4" t="s">
         <v>72</v>
       </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -704,6 +710,9 @@
       <c r="E5" t="s">
         <v>72</v>
       </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -721,6 +730,9 @@
       <c r="E6" t="s">
         <v>72</v>
       </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -738,6 +750,9 @@
       <c r="E7" t="s">
         <v>72</v>
       </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -755,6 +770,9 @@
       <c r="E8" t="s">
         <v>72</v>
       </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -772,6 +790,9 @@
       <c r="E9" t="s">
         <v>70</v>
       </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -789,6 +810,9 @@
       <c r="E10" t="s">
         <v>70</v>
       </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -806,6 +830,9 @@
       <c r="E11" t="s">
         <v>72</v>
       </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -823,6 +850,9 @@
       <c r="E12" t="s">
         <v>72</v>
       </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -840,6 +870,9 @@
       <c r="E13" t="s">
         <v>70</v>
       </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -857,6 +890,9 @@
       <c r="E14" t="s">
         <v>70</v>
       </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -874,6 +910,9 @@
       <c r="E15" t="s">
         <v>72</v>
       </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -891,8 +930,11 @@
       <c r="E16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -908,8 +950,11 @@
       <c r="E17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -925,8 +970,11 @@
       <c r="E18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -942,8 +990,11 @@
       <c r="E19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -959,8 +1010,11 @@
       <c r="E20" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -976,8 +1030,11 @@
       <c r="E21" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -993,8 +1050,11 @@
       <c r="E22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1010,8 +1070,11 @@
       <c r="E23" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1027,8 +1090,11 @@
       <c r="E24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1044,8 +1110,11 @@
       <c r="E25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1061,8 +1130,11 @@
       <c r="E26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1078,8 +1150,11 @@
       <c r="E27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1095,8 +1170,11 @@
       <c r="E28" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1112,8 +1190,11 @@
       <c r="E29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1129,8 +1210,11 @@
       <c r="E30" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1146,8 +1230,11 @@
       <c r="E31" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1163,8 +1250,11 @@
       <c r="E32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1180,8 +1270,11 @@
       <c r="E33" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1197,8 +1290,11 @@
       <c r="E34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1214,8 +1310,11 @@
       <c r="E35" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1231,8 +1330,11 @@
       <c r="E36" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1248,8 +1350,11 @@
       <c r="E37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1265,8 +1370,11 @@
       <c r="E38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1282,8 +1390,11 @@
       <c r="E39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1299,8 +1410,11 @@
       <c r="E40" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1316,8 +1430,11 @@
       <c r="E41" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1333,8 +1450,11 @@
       <c r="E42" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -1350,8 +1470,11 @@
       <c r="E43" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -1367,8 +1490,11 @@
       <c r="E44" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>78</v>
       </c>
@@ -1384,8 +1510,11 @@
       <c r="E45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -1401,8 +1530,11 @@
       <c r="E46" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -1418,8 +1550,11 @@
       <c r="E47" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -1435,8 +1570,11 @@
       <c r="E48" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -1452,8 +1590,11 @@
       <c r="E49" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -1469,8 +1610,11 @@
       <c r="E50" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -1486,8 +1630,11 @@
       <c r="E51" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -1503,8 +1650,11 @@
       <c r="E52" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -1520,8 +1670,11 @@
       <c r="E53" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1537,8 +1690,11 @@
       <c r="E54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -1554,8 +1710,11 @@
       <c r="E55" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1571,8 +1730,11 @@
       <c r="E56" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1588,8 +1750,11 @@
       <c r="E57" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1605,8 +1770,11 @@
       <c r="E58" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1622,8 +1790,11 @@
       <c r="E59" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1639,8 +1810,11 @@
       <c r="E60" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -1656,13 +1830,16 @@
       <c r="E61" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -1678,8 +1855,11 @@
       <c r="E64" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -1695,8 +1875,11 @@
       <c r="E65" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>13</v>
       </c>
@@ -1712,8 +1895,11 @@
       <c r="E66" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -1729,8 +1915,11 @@
       <c r="E67" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>21</v>
       </c>
@@ -1746,8 +1935,11 @@
       <c r="E68" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>27</v>
       </c>
@@ -1763,8 +1955,11 @@
       <c r="E69" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -1780,8 +1975,11 @@
       <c r="E70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>29</v>
       </c>
@@ -1797,8 +1995,11 @@
       <c r="E71" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -1814,8 +2015,11 @@
       <c r="E72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>53</v>
       </c>
@@ -1831,8 +2035,11 @@
       <c r="E73" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -1848,8 +2055,11 @@
       <c r="E74" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>54</v>
       </c>
@@ -1865,8 +2075,11 @@
       <c r="E75" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -1882,8 +2095,11 @@
       <c r="E76" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -1898,6 +2114,9 @@
       </c>
       <c r="E77" t="s">
         <v>72</v>
+      </c>
+      <c r="F77" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked through chapter 6
Also added packages from all previous chapters to index that were missed
before
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68AE027A-8891-46E5-97E0-31B6824F485E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9C3282FA-3438-49CB-BCB8-BD6B914F2BAC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="87">
   <si>
     <t>Index terms</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>pdata</t>
+  </si>
+  <si>
+    <t>Residuals vs Leverage</t>
+  </si>
+  <si>
+    <t>validity conditions</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -673,6 +679,9 @@
       <c r="F3" t="s">
         <v>70</v>
       </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -693,6 +702,9 @@
       <c r="F4" t="s">
         <v>70</v>
       </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -713,6 +725,9 @@
       <c r="F5" t="s">
         <v>70</v>
       </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -733,6 +748,9 @@
       <c r="F6" t="s">
         <v>70</v>
       </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -753,6 +771,9 @@
       <c r="F7" t="s">
         <v>72</v>
       </c>
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -773,6 +794,9 @@
       <c r="F8" t="s">
         <v>70</v>
       </c>
+      <c r="G8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -793,6 +817,9 @@
       <c r="F9" t="s">
         <v>70</v>
       </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -813,6 +840,9 @@
       <c r="F10" t="s">
         <v>70</v>
       </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -833,6 +863,9 @@
       <c r="F11" t="s">
         <v>70</v>
       </c>
+      <c r="G11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -853,6 +886,9 @@
       <c r="F12" t="s">
         <v>70</v>
       </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -873,6 +909,9 @@
       <c r="F13" t="s">
         <v>70</v>
       </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -893,6 +932,9 @@
       <c r="F14" t="s">
         <v>70</v>
       </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -913,6 +955,9 @@
       <c r="F15" t="s">
         <v>70</v>
       </c>
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -933,8 +978,11 @@
       <c r="F16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -953,8 +1001,11 @@
       <c r="F17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -973,8 +1024,11 @@
       <c r="F18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -993,8 +1047,11 @@
       <c r="F19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1013,8 +1070,11 @@
       <c r="F20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1033,8 +1093,11 @@
       <c r="F21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1053,8 +1116,11 @@
       <c r="F22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1073,8 +1139,11 @@
       <c r="F23" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1093,8 +1162,11 @@
       <c r="F24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1113,8 +1185,11 @@
       <c r="F25" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1133,8 +1208,11 @@
       <c r="F26" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1153,8 +1231,11 @@
       <c r="F27" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1173,8 +1254,11 @@
       <c r="F28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1193,8 +1277,11 @@
       <c r="F29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1213,8 +1300,11 @@
       <c r="F30" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1233,8 +1323,11 @@
       <c r="F31" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1253,8 +1346,11 @@
       <c r="F32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1273,8 +1369,11 @@
       <c r="F33" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1293,8 +1392,11 @@
       <c r="F34" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1313,8 +1415,11 @@
       <c r="F35" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1333,8 +1438,11 @@
       <c r="F36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1353,8 +1461,11 @@
       <c r="F37" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1373,8 +1484,11 @@
       <c r="F38" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1393,729 +1507,886 @@
       <c r="F39" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>76</v>
       </c>
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E43" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>77</v>
       </c>
-      <c r="B44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" t="s">
-        <v>70</v>
-      </c>
-      <c r="F44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" t="s">
+        <v>70</v>
+      </c>
+      <c r="G45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>79</v>
       </c>
-      <c r="B46" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" t="s">
-        <v>70</v>
-      </c>
-      <c r="F46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>80</v>
       </c>
-      <c r="B47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" t="s">
-        <v>70</v>
-      </c>
-      <c r="F47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>81</v>
       </c>
-      <c r="B48" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" t="s">
+        <v>70</v>
+      </c>
+      <c r="G49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>82</v>
       </c>
-      <c r="B49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" t="s">
-        <v>70</v>
-      </c>
-      <c r="F49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" t="s">
+        <v>70</v>
+      </c>
+      <c r="G50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>83</v>
       </c>
-      <c r="B50" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" t="s">
-        <v>72</v>
-      </c>
-      <c r="E50" t="s">
-        <v>70</v>
-      </c>
-      <c r="F50" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" t="s">
+        <v>70</v>
+      </c>
+      <c r="G51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>46</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>71</v>
       </c>
-      <c r="C51" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" t="s">
-        <v>72</v>
-      </c>
-      <c r="F51" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+      <c r="C52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" t="s">
+        <v>72</v>
+      </c>
+      <c r="F52" t="s">
+        <v>70</v>
+      </c>
+      <c r="G52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B52" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" t="s">
-        <v>72</v>
-      </c>
-      <c r="F52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>48</v>
       </c>
-      <c r="B53" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" t="s">
-        <v>72</v>
-      </c>
-      <c r="F53" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" t="s">
+        <v>70</v>
+      </c>
+      <c r="G54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>49</v>
       </c>
-      <c r="B54" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" t="s">
-        <v>70</v>
-      </c>
-      <c r="F54" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" t="s">
+        <v>70</v>
+      </c>
+      <c r="F55" t="s">
+        <v>72</v>
+      </c>
+      <c r="G55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>50</v>
       </c>
-      <c r="B55" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" t="s">
-        <v>72</v>
-      </c>
-      <c r="D55" t="s">
-        <v>70</v>
-      </c>
-      <c r="E55" t="s">
-        <v>72</v>
-      </c>
-      <c r="F55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" t="s">
+        <v>72</v>
+      </c>
+      <c r="G56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>51</v>
       </c>
-      <c r="B56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" t="s">
-        <v>72</v>
-      </c>
-      <c r="E57" t="s">
-        <v>70</v>
-      </c>
-      <c r="F57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" t="s">
+        <v>70</v>
+      </c>
+      <c r="G58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" t="s">
-        <v>72</v>
-      </c>
-      <c r="E58" t="s">
-        <v>72</v>
-      </c>
-      <c r="F58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>72</v>
+      </c>
+      <c r="E59" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" t="s">
+        <v>70</v>
+      </c>
+      <c r="G59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" t="s">
+        <v>72</v>
+      </c>
+      <c r="G60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59" t="s">
-        <v>72</v>
-      </c>
-      <c r="E59" t="s">
-        <v>70</v>
-      </c>
-      <c r="F59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" t="s">
+        <v>70</v>
+      </c>
+      <c r="G61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" t="s">
-        <v>70</v>
-      </c>
-      <c r="D60" t="s">
-        <v>72</v>
-      </c>
-      <c r="E60" t="s">
-        <v>70</v>
-      </c>
-      <c r="F60" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E62" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>73</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>71</v>
       </c>
-      <c r="C61" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" t="s">
-        <v>70</v>
-      </c>
-      <c r="E61" t="s">
-        <v>70</v>
-      </c>
-      <c r="F61" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A63" s="1" t="s">
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
         <v>11</v>
       </c>
-      <c r="B64" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D64" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" t="s">
-        <v>72</v>
-      </c>
-      <c r="F64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" t="s">
+        <v>70</v>
+      </c>
+      <c r="G66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>12</v>
       </c>
-      <c r="B65" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" t="s">
-        <v>70</v>
-      </c>
-      <c r="D65" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" t="s">
-        <v>72</v>
-      </c>
-      <c r="F65" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" t="s">
+        <v>70</v>
+      </c>
+      <c r="G67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>13</v>
       </c>
-      <c r="B66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" t="s">
-        <v>72</v>
-      </c>
-      <c r="E66" t="s">
-        <v>72</v>
-      </c>
-      <c r="F66" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68" t="s">
+        <v>72</v>
+      </c>
+      <c r="F68" t="s">
+        <v>70</v>
+      </c>
+      <c r="G68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>14</v>
       </c>
-      <c r="B67" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" t="s">
-        <v>70</v>
-      </c>
-      <c r="D67" t="s">
-        <v>72</v>
-      </c>
-      <c r="E67" t="s">
-        <v>72</v>
-      </c>
-      <c r="F67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" t="s">
+        <v>72</v>
+      </c>
+      <c r="E69" t="s">
+        <v>72</v>
+      </c>
+      <c r="F69" t="s">
+        <v>70</v>
+      </c>
+      <c r="G69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>21</v>
       </c>
-      <c r="B68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" t="s">
-        <v>70</v>
-      </c>
-      <c r="D68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E68" t="s">
-        <v>72</v>
-      </c>
-      <c r="F68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
+        <v>72</v>
+      </c>
+      <c r="E70" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" t="s">
+        <v>70</v>
+      </c>
+      <c r="G70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>27</v>
       </c>
-      <c r="B69" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" t="s">
-        <v>70</v>
-      </c>
-      <c r="D69" t="s">
-        <v>70</v>
-      </c>
-      <c r="E69" t="s">
-        <v>72</v>
-      </c>
-      <c r="F69" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F71" t="s">
+        <v>70</v>
+      </c>
+      <c r="G71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>28</v>
       </c>
-      <c r="B70" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" t="s">
-        <v>70</v>
-      </c>
-      <c r="D70" t="s">
-        <v>70</v>
-      </c>
-      <c r="E70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" t="s">
+        <v>70</v>
+      </c>
+      <c r="F72" t="s">
+        <v>72</v>
+      </c>
+      <c r="G72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>29</v>
       </c>
-      <c r="B71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>70</v>
-      </c>
-      <c r="D71" t="s">
-        <v>72</v>
-      </c>
-      <c r="E71" t="s">
-        <v>72</v>
-      </c>
-      <c r="F71" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+      <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="s">
+        <v>70</v>
+      </c>
+      <c r="D73" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" t="s">
+        <v>72</v>
+      </c>
+      <c r="F73" t="s">
+        <v>72</v>
+      </c>
+      <c r="G73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
         <v>52</v>
       </c>
-      <c r="B72" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" t="s">
-        <v>72</v>
-      </c>
-      <c r="E72" t="s">
-        <v>72</v>
-      </c>
-      <c r="F72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
+      <c r="B74" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" t="s">
+        <v>70</v>
+      </c>
+      <c r="D74" t="s">
+        <v>72</v>
+      </c>
+      <c r="E74" t="s">
+        <v>72</v>
+      </c>
+      <c r="F74" t="s">
+        <v>70</v>
+      </c>
+      <c r="G74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
         <v>53</v>
       </c>
-      <c r="B73" t="s">
-        <v>70</v>
-      </c>
-      <c r="C73" t="s">
-        <v>72</v>
-      </c>
-      <c r="D73" t="s">
-        <v>70</v>
-      </c>
-      <c r="E73" t="s">
-        <v>70</v>
-      </c>
-      <c r="F73" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+      <c r="B75" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s">
+        <v>70</v>
+      </c>
+      <c r="E75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F75" t="s">
+        <v>70</v>
+      </c>
+      <c r="G75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
         <v>84</v>
       </c>
-      <c r="B74" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" t="s">
-        <v>70</v>
-      </c>
-      <c r="F74" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
+      <c r="B76" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" t="s">
+        <v>72</v>
+      </c>
+      <c r="G76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>54</v>
       </c>
-      <c r="B75" t="s">
-        <v>70</v>
-      </c>
-      <c r="C75" t="s">
-        <v>70</v>
-      </c>
-      <c r="D75" t="s">
-        <v>70</v>
-      </c>
-      <c r="E75" t="s">
-        <v>70</v>
-      </c>
-      <c r="F75" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
+      <c r="B77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C77" t="s">
+        <v>70</v>
+      </c>
+      <c r="D77" t="s">
+        <v>70</v>
+      </c>
+      <c r="E77" t="s">
+        <v>70</v>
+      </c>
+      <c r="F77" t="s">
+        <v>72</v>
+      </c>
+      <c r="G77" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>19</v>
       </c>
-      <c r="B76" t="s">
-        <v>70</v>
-      </c>
-      <c r="C76" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76" t="s">
-        <v>70</v>
-      </c>
-      <c r="E76" t="s">
-        <v>70</v>
-      </c>
-      <c r="F76" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
+      <c r="B78" t="s">
+        <v>70</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" t="s">
+        <v>70</v>
+      </c>
+      <c r="E78" t="s">
+        <v>70</v>
+      </c>
+      <c r="F78" t="s">
+        <v>70</v>
+      </c>
+      <c r="G78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>55</v>
       </c>
-      <c r="B77" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" t="s">
-        <v>70</v>
-      </c>
-      <c r="D77" t="s">
-        <v>70</v>
-      </c>
-      <c r="E77" t="s">
-        <v>72</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="B79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79" t="s">
+        <v>70</v>
+      </c>
+      <c r="D79" t="s">
+        <v>70</v>
+      </c>
+      <c r="E79" t="s">
+        <v>72</v>
+      </c>
+      <c r="F79" t="s">
+        <v>70</v>
+      </c>
+      <c r="G79" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added index terms to chapter 8, added a few more index terms to chapters 6 and 7. Adjusted layout of chapter 8.
scatterplot() legends needed to be adjusted for a couple plots
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D562C6D-A72B-4B00-AD75-A0554B889613}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{61849D01-7521-4F27-8DEE-6AFE07D1FE7A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="90">
   <si>
     <t>Index terms</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>R packages</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n/a</t>
   </si>
 </sst>
 </file>
@@ -620,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -691,6 +694,9 @@
       <c r="H3" t="s">
         <v>70</v>
       </c>
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -717,6 +723,9 @@
       <c r="H4" t="s">
         <v>70</v>
       </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -743,6 +752,9 @@
       <c r="H5" t="s">
         <v>70</v>
       </c>
+      <c r="I5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -769,6 +781,9 @@
       <c r="H6" t="s">
         <v>70</v>
       </c>
+      <c r="I6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -795,6 +810,9 @@
       <c r="H7" t="s">
         <v>72</v>
       </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -821,6 +839,9 @@
       <c r="H8" t="s">
         <v>70</v>
       </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -847,6 +868,9 @@
       <c r="H9" t="s">
         <v>72</v>
       </c>
+      <c r="I9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -873,6 +897,9 @@
       <c r="H10" t="s">
         <v>70</v>
       </c>
+      <c r="I10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -899,6 +926,9 @@
       <c r="H11" t="s">
         <v>70</v>
       </c>
+      <c r="I11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -925,6 +955,9 @@
       <c r="H12" t="s">
         <v>70</v>
       </c>
+      <c r="I12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -951,6 +984,9 @@
       <c r="H13" t="s">
         <v>70</v>
       </c>
+      <c r="I13" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -977,6 +1013,9 @@
       <c r="H14" t="s">
         <v>70</v>
       </c>
+      <c r="I14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -1003,6 +1042,9 @@
       <c r="H15" t="s">
         <v>70</v>
       </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -1029,8 +1071,11 @@
       <c r="H16" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1055,8 +1100,11 @@
       <c r="H17" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1081,8 +1129,11 @@
       <c r="H18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1107,8 +1158,11 @@
       <c r="H19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1133,8 +1187,11 @@
       <c r="H20" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1159,8 +1216,11 @@
       <c r="H21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1185,8 +1245,11 @@
       <c r="H22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1211,8 +1274,11 @@
       <c r="H23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1237,8 +1303,11 @@
       <c r="H24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1263,8 +1332,11 @@
       <c r="H25" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1289,8 +1361,11 @@
       <c r="H26" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1315,8 +1390,11 @@
       <c r="H27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1341,8 +1419,11 @@
       <c r="H28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1367,8 +1448,11 @@
       <c r="H29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1393,8 +1477,11 @@
       <c r="H30" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1419,8 +1506,11 @@
       <c r="H31" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1445,8 +1535,11 @@
       <c r="H32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1471,8 +1564,11 @@
       <c r="H33" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1497,8 +1593,11 @@
       <c r="H34" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1523,8 +1622,11 @@
       <c r="H35" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1549,8 +1651,11 @@
       <c r="H36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1575,8 +1680,11 @@
       <c r="H37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1601,8 +1709,11 @@
       <c r="H38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1627,8 +1738,11 @@
       <c r="H39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1653,8 +1767,11 @@
       <c r="H40" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1679,8 +1796,11 @@
       <c r="H41" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1705,8 +1825,11 @@
       <c r="H42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1731,8 +1854,11 @@
       <c r="H43" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1757,8 +1883,11 @@
       <c r="H44" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -1783,8 +1912,11 @@
       <c r="H45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -1809,8 +1941,11 @@
       <c r="H46" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1835,8 +1970,11 @@
       <c r="H47" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -1861,8 +1999,11 @@
       <c r="H48" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -1887,8 +2028,11 @@
       <c r="H49" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>81</v>
       </c>
@@ -1913,8 +2057,11 @@
       <c r="H50" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -1939,8 +2086,11 @@
       <c r="H51" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -1965,8 +2115,11 @@
       <c r="H52" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -1991,8 +2144,11 @@
       <c r="H53" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -2017,8 +2173,11 @@
       <c r="H54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2043,8 +2202,11 @@
       <c r="H55" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -2069,8 +2231,11 @@
       <c r="H56" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -2095,8 +2260,11 @@
       <c r="H57" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2121,8 +2289,11 @@
       <c r="H58" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -2147,8 +2318,11 @@
       <c r="H59" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -2173,8 +2347,11 @@
       <c r="H60" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -2199,8 +2376,11 @@
       <c r="H61" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -2225,8 +2405,11 @@
       <c r="H62" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -2251,8 +2434,11 @@
       <c r="H63" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -2277,13 +2463,16 @@
       <c r="H64" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -2308,8 +2497,11 @@
       <c r="H67" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -2334,8 +2526,11 @@
       <c r="H68" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -2360,8 +2555,11 @@
       <c r="H69" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -2386,8 +2584,11 @@
       <c r="H70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -2412,8 +2613,11 @@
       <c r="H71" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>27</v>
       </c>
@@ -2438,8 +2642,11 @@
       <c r="H72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -2464,8 +2671,11 @@
       <c r="H73" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -2490,8 +2700,11 @@
       <c r="H74" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2516,8 +2729,11 @@
       <c r="H75" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -2542,8 +2758,11 @@
       <c r="H76" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I76" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -2568,8 +2787,11 @@
       <c r="H77" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I77" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>54</v>
       </c>
@@ -2594,8 +2816,11 @@
       <c r="H78" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2620,8 +2845,11 @@
       <c r="H79" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -2644,6 +2872,9 @@
         <v>70</v>
       </c>
       <c r="H80" t="s">
+        <v>70</v>
+      </c>
+      <c r="I80" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edits up to 2.2
Changes up to 2.2 with some index additions and small writing changes.
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greta\Documents\Greenwood_book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w76c139\Box Sync\Greenwood_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{61849D01-7521-4F27-8DEE-6AFE07D1FE7A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PossibleOtherTerms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="117">
   <si>
     <t>Index terms</t>
   </si>
@@ -295,12 +295,93 @@
   </si>
   <si>
     <t xml:space="preserve"> n/a</t>
+  </si>
+  <si>
+    <t>Quantitative variable</t>
+  </si>
+  <si>
+    <t>Categorical variable</t>
+  </si>
+  <si>
+    <t>Response variable</t>
+  </si>
+  <si>
+    <t>Explanatory variable</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>5 number summary</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>histogram</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>tibble</t>
+  </si>
+  <si>
+    <t>causal effect</t>
+  </si>
+  <si>
+    <t>outlier</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>density curve</t>
+  </si>
+  <si>
+    <t>rug</t>
+  </si>
+  <si>
+    <t>jitter</t>
+  </si>
+  <si>
+    <t>boxplot</t>
+  </si>
+  <si>
+    <t>Already indexed?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>tilde</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,24 +701,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +750,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -698,7 +779,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -727,7 +808,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -756,7 +837,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -785,7 +866,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -814,7 +895,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -843,7 +924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -872,7 +953,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -901,7 +982,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -930,7 +1011,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -959,7 +1040,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -988,7 +1069,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1017,7 +1098,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1046,7 +1127,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1075,7 +1156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1104,7 +1185,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1133,7 +1214,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1162,7 +1243,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1191,7 +1272,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1220,7 +1301,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1249,7 +1330,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1359,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1307,7 +1388,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1336,7 +1417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1365,7 +1446,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1394,7 +1475,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1423,7 +1504,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1452,7 +1533,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1481,7 +1562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1510,7 +1591,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1539,7 +1620,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1568,7 +1649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1597,7 +1678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1626,7 +1707,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1655,7 +1736,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1684,7 +1765,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1794,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1742,7 +1823,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1771,7 +1852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1800,7 +1881,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1829,7 +1910,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1858,7 +1939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1887,7 +1968,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -1916,7 +1997,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -1945,7 +2026,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -1974,7 +2055,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -2003,7 +2084,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -2032,7 +2113,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>81</v>
       </c>
@@ -2061,7 +2142,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -2090,7 +2171,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -2119,7 +2200,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -2148,7 +2229,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -2177,7 +2258,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2206,7 +2287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -2235,7 +2316,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -2264,7 +2345,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -2293,7 +2374,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -2322,7 +2403,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -2351,7 +2432,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -2380,7 +2461,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -2409,7 +2490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -2438,7 +2519,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -2467,12 +2548,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -2501,7 +2582,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -2530,7 +2611,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -2559,7 +2640,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -2588,7 +2669,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -2617,7 +2698,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>27</v>
       </c>
@@ -2646,7 +2727,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -2675,7 +2756,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -2704,7 +2785,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2733,7 +2814,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>53</v>
       </c>
@@ -2762,7 +2843,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -2791,7 +2872,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>54</v>
       </c>
@@ -2820,7 +2901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2849,7 +2930,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -2878,7 +2959,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>88</v>
       </c>
@@ -2887,4 +2968,266 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="L20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Getting close on 5.0
More index edits and small other changes throughout.
</commit_message>
<xml_diff>
--- a/TermsForIndex.xlsx
+++ b/TermsForIndex.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="129">
   <si>
     <t>Index terms</t>
   </si>
@@ -376,6 +376,42 @@
   </si>
   <si>
     <t>standard deviation</t>
+  </si>
+  <si>
+    <t>term plot</t>
+  </si>
+  <si>
+    <t>VIF</t>
+  </si>
+  <si>
+    <t>vif</t>
+  </si>
+  <si>
+    <t>correlation plot</t>
+  </si>
+  <si>
+    <t>seq</t>
+  </si>
+  <si>
+    <t>F-test - overall</t>
+  </si>
+  <si>
+    <t>Tukey's HSD</t>
+  </si>
+  <si>
+    <t>family-wise error rate</t>
+  </si>
+  <si>
+    <t>CLD</t>
+  </si>
+  <si>
+    <t>replicate</t>
+  </si>
+  <si>
+    <t>indicator variable</t>
+  </si>
+  <si>
+    <t>model!nested</t>
   </si>
 </sst>
 </file>
@@ -704,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:J2"/>
     </sheetView>
   </sheetViews>
@@ -2972,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,24 +3242,131 @@
         <v>113</v>
       </c>
     </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>123</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="I33" t="s">
+        <v>96</v>
+      </c>
+      <c r="J33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>107</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="I40" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>